<commit_message>
test with aip bugs fixed
</commit_message>
<xml_diff>
--- a/media/predictions.xlsx
+++ b/media/predictions.xlsx
@@ -34,7 +34,7 @@
     <t>appropriate</t>
   </si>
   <si>
-    <t>0.9989719390869141</t>
+    <t>1.0000100135803223</t>
   </si>
   <si>
     <t>fasttext filter</t>
@@ -55,37 +55,37 @@
     <t>×ساریناهستم× ^۱۳ سالمه^ ←عشق خودمم→</t>
   </si>
   <si>
-    <t>0.9823118448257446</t>
+    <t>0.9999911785125732</t>
   </si>
   <si>
     <t>دوستت دارمk😘😘😘ولی حیف که نیستی</t>
   </si>
   <si>
-    <t>0.9441972374916077</t>
+    <t>0.9993734955787659</t>
   </si>
   <si>
     <t xml:space="preserve">صــلـ ــم... :) حالــتـ ــچطورع...!؟  فالــو کـن فالــ ــو میـشیـ </t>
   </si>
   <si>
-    <t>0.9734523296356201</t>
+    <t>0.9995195865631104</t>
   </si>
   <si>
     <t>منیم جان ج یارمسان دا نفسیم..عشقم من برم خیلی دیر وقته الانم یواشکی دارم ج میدم خیلییی دوست دارم من بوسس ر ولپات زندگیم مراقب خودت باش جون و دلم شبتخوش عزیزم</t>
   </si>
   <si>
-    <t>0.8389291763305664</t>
+    <t>0.9763948917388916</t>
   </si>
   <si>
     <t>⁑☾˙❀‿❀˙☽⁑هانیتا هستم ⁑☾˙❀‿❀˙☽⁑    ۱۳ سالمه♡😉 🖤‌███████]99% (｡♡‿♡｡)   ( ˘ ³˘)❤  بزنــــ رویـ نمایشـ همـــــــهـ (*＾3＾)♡  ( ˘ ³˘)❤ (◍•ᴗ•◍)♥  (⑉°з°)-♡  مرسیــ از دنــبال کننــده هام 😍❤ (◍•ᴗ•◍)✧</t>
   </si>
   <si>
-    <t>0.9562497138977051</t>
+    <t>0.991457462310791</t>
   </si>
   <si>
     <t xml:space="preserve">                         مقدار یار همنفس ؛ چون من نداند هیچکس...   ماهی که بر خشک افتد؛قیمت بداند آب را....🙃🍂                  🥀                  </t>
   </si>
   <si>
-    <t>0.9568185210227966</t>
+    <t>0.9991353154182434</t>
   </si>
   <si>
     <t>من پسرک تنها هستم 😔 آیدی روبیکا PosarkTANHA@ آیدی شاد POSARKA01@ آیدی تلگرام SYBER19@ اگه خواستید اس بدید منتظرم  مخصوصاً دخترا 😘</t>
@@ -97,61 +97,61 @@
     <t xml:space="preserve">سلام من متین هستم ۱۲ سالمه عاشق بازی های ویدویی هستم </t>
   </si>
   <si>
-    <t>0.9863117933273315</t>
+    <t>0.9991846680641174</t>
   </si>
   <si>
     <t>سلام ....😐😐😐  ی دختر خوشگل و جذاب😛😛😛  تیر ماهی،پرسپولیسی❤❤❤  فالوم کنید ترو خدا من به هزار برسم😘🙏</t>
   </si>
   <si>
-    <t>0.858184814453125</t>
+    <t>0.952233612537384</t>
   </si>
   <si>
     <t>من هیولا نیستم... من فقط‌یه وضعیت بحرانی ام... $$$$$$$$</t>
   </si>
   <si>
-    <t>0.9569402933120728</t>
+    <t>0.9980811476707458</t>
   </si>
   <si>
     <t xml:space="preserve">                         مقدار یار همنفس ؛ چون من نداند هیچکس...   ماهی که بر خشک افتد؛قیمت بداند آب را....🙃🍂  #سعدی                🥀                  </t>
   </si>
   <si>
-    <t>0.9446946978569031</t>
+    <t>0.9981659054756165</t>
   </si>
   <si>
     <t>باشه اومدم.بغلت.بغل گرمتو دوس دارم</t>
   </si>
   <si>
-    <t>0.8305115103721619</t>
+    <t>0.9970064163208008</t>
   </si>
   <si>
     <t>🐞سلام🐞 🐞اسم:مایسا🐞 🐞سن:10🐞 🐞برنامه کودک مورد علاقه:لیدی باگ🐞 🐞فیلم مورد علاقه:سیب ممنوعه🐞 هرکی لیدی باگ رو دوست داره فالو کنه😌 ورود پسر هم ممنوع🚫 بجوز فامیل ها😌 ف</t>
   </si>
   <si>
-    <t>0.8287726640701294</t>
+    <t>0.9297232031822205</t>
   </si>
   <si>
     <t>༒ᴾᴵᴿᵉ ᴹᴬᴶᴬᶻᴵ༒  🍷ᵈᴼᶜᵗᵒʳ ᵛⁱʳᵒˢ🍷   ⊱tчpєr αzαm⊰           بـــزݩـ نمایــــش همہ</t>
   </si>
   <si>
-    <t>0.8720709681510925</t>
+    <t>0.9919484257698059</t>
   </si>
   <si>
     <t>هیچوقت نمیفهمی چقدر قوی هستی.. تا اینکه قوی بودن تنها انتخابت باشه!</t>
   </si>
   <si>
-    <t>0.952329695224762</t>
+    <t>0.9998220801353455</t>
   </si>
   <si>
     <t>من پرسپولیسی هستم 👑عاشق پارس ELX و ۴۰۵وسمند😘😝😎♠</t>
   </si>
   <si>
-    <t>0.9415902495384216</t>
+    <t>0.998589277267456</t>
   </si>
   <si>
     <t>"bu ɦaყat heycan meycan ყʊk" ٬ "bu ɦaყat heycan meycan ყʊk"   ٬   →"ყʊk"←        &amp;lt;• • •&amp;gt;  →çokur←       "kazaŋ ٬ kazaŋ (ყʊk)"       lℳ gɨrl←✨     نآمزدم😹↩«🌸ݐـاصتـامـہ🌸»     ↑</t>
   </si>
   <si>
-    <t>0.9629700779914856</t>
+    <t>0.9988031387329102</t>
   </si>
 </sst>
 </file>

</xml_diff>